<commit_message>
Excel angepasst, Testdateien (Jakob) gelöscht
</commit_message>
<xml_diff>
--- a/MeritOrder_Excel.xlsx
+++ b/MeritOrder_Excel.xlsx
@@ -1,29 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="113_{91C7DA48-37B9-45B2-AB4B-E86EEFD7DA94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4F8D0A05-C2C0-42D9-99BC-8DB41A49435D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA96C01-6E1C-4383-A57E-8FCC76A4AE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kraftwerke" sheetId="4" r:id="rId1"/>
-    <sheet name="Leistung" sheetId="1" r:id="rId2"/>
+    <sheet name="Cockpit" sheetId="5" r:id="rId1"/>
+    <sheet name="Kraftwerke" sheetId="4" r:id="rId2"/>
     <sheet name="Kosten" sheetId="2" r:id="rId3"/>
-    <sheet name="Nachfrage" sheetId="3" r:id="rId4"/>
+    <sheet name="Kapazität" sheetId="1" r:id="rId4"/>
+    <sheet name="Nachfrage" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>var_cost</t>
   </si>
@@ -67,14 +78,257 @@
     <t>Kraftwerkstyp</t>
   </si>
   <si>
-    <t>Zeit</t>
+    <t>Stunde</t>
+  </si>
+  <si>
+    <t>Erdgas</t>
+  </si>
+  <si>
+    <t>Braunkohle</t>
+  </si>
+  <si>
+    <t>Steinkohle</t>
+  </si>
+  <si>
+    <r>
+      <t>Brennstoffkosten [€/MWh</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-Preis [€/Tonne CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>EU ETS</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <t>Emissionsfaktoren [t CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / MWh</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Grenzkosten [€/MWh</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>el</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Variable Inputfaktoren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berechnete Werte </t>
+  </si>
+  <si>
+    <t>Fixe Inputfaktoren</t>
+  </si>
+  <si>
+    <r>
+      <t>Wirkungsgrade [MWh</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>el</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/MWh</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Inputparameter Merit-Order-Modell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,16 +336,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -99,14 +403,131 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,11 +805,292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9F5ADF-242F-44CD-878A-25895C987D0F}">
+  <dimension ref="B2:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="6.53125" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="23"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="8">
+        <v>54.06</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="5"/>
+      <c r="C17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="15">
+        <v>0.54</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0.51</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="17">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="17">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="18">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="19">
+        <f>$C$9/$C$18+$C$23/$C$18*$C$14</f>
+        <v>61.427848101265816</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="19">
+        <f>$C$9/$D$18+$C$23/$D$18*$C$14</f>
+        <v>70.127167630057798</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="19">
+        <f>$C$9/$E$18+$C$23/$E$18*$C$14</f>
+        <v>78.779220779220779</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="19">
+        <f>$C$10/$C$19+$C$24/$C$19*$C$14</f>
+        <v>82.210796915167094</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="19">
+        <f>$C$10/$D$19+$C$24/$D$19*$C$14</f>
+        <v>95.462686567164184</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="19">
+        <f>$C$10/$E$19+$C$24/$E$19*$C$14</f>
+        <v>108.40677966101696</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="19">
+        <f>$C$11/$C$20+$C$25/$C$20*$C$14</f>
+        <v>119.56296296296297</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="19">
+        <f>$C$11/$D$20+$C$25/$D$20*$C$14</f>
+        <v>126.59607843137255</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="20">
+        <f>$C$11/$E$20+$C$25/$E$20*$C$14</f>
+        <v>140.35652173913044</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462A2DE2-E034-4F83-9F51-3596A9040BF8}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -456,7 +1158,87 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA14E8B2-0A04-4EA8-A66C-564981641E2D}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <f>Cockpit!C28</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
+        <f>Cockpit!C29</f>
+        <v>61.427848101265816</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="2">
+        <f>Cockpit!C30</f>
+        <v>70.127167630057798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
+        <f>Cockpit!C31</f>
+        <v>78.779220779220779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
+        <f>Cockpit!C32</f>
+        <v>82.210796915167094</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <f>Cockpit!C33</f>
+        <v>95.462686567164184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
+        <f>Cockpit!C34</f>
+        <v>108.40677966101696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" s="2">
+        <f>Cockpit!C35</f>
+        <v>119.56296296296297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" s="2">
+        <f>Cockpit!C36</f>
+        <v>126.59607843137255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" s="2">
+        <f>Cockpit!C37</f>
+        <v>140.35652173913044</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -527,82 +1309,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA14E8B2-0A04-4EA8-A66C-564981641E2D}">
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>140</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503AA485-0496-4332-9891-D6E32C8F4635}">
   <dimension ref="A1:B8761"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8754" sqref="G8754"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Constraints über zweidimensionale sets definiert bzw umgeschrieben
</commit_message>
<xml_diff>
--- a/MeritOrder_Excel.xlsx
+++ b/MeritOrder_Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="102_{63E64240-B49F-4893-92D0-7310A5C95277}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EAA4D83-33F6-4C30-83C1-07A85CBF7C2F}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="113_{3DCE0A75-BC1E-4D96-98EA-373A843AE2DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{E28DB717-1D86-48F0-ABE8-3718FCCB22AC}"/>
   <bookViews>
     <workbookView xWindow="7500" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1314,7 +1314,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Diese Version nicht wieder verwenden
</commit_message>
<xml_diff>
--- a/MeritOrder_Excel.xlsx
+++ b/MeritOrder_Excel.xlsx
@@ -3,44 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="113_{3DCE0A75-BC1E-4D96-98EA-373A843AE2DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{E28DB717-1D86-48F0-ABE8-3718FCCB22AC}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{05169759-1DF6-4B85-9889-E7106E068EC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9D3482BE-EB4F-467A-BD05-84B5A3DB3C61}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cockpit" sheetId="5" r:id="rId1"/>
     <sheet name="Kraftwerke" sheetId="4" r:id="rId2"/>
-    <sheet name="Kosten" sheetId="2" r:id="rId3"/>
-    <sheet name="Kapazität" sheetId="1" r:id="rId4"/>
-    <sheet name="Nachfrage" sheetId="3" r:id="rId5"/>
+    <sheet name="Brennstoffe" sheetId="6" r:id="rId3"/>
+    <sheet name="Nachfrage" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
-  <si>
-    <t>var_cost</t>
-  </si>
-  <si>
-    <t>Leistung</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Nachfrage</t>
   </si>
@@ -73,9 +56,6 @@
   </si>
   <si>
     <t>Erdgas (-)</t>
-  </si>
-  <si>
-    <t>Kraftwerkstyp</t>
   </si>
   <si>
     <t>Stunde</t>
@@ -318,6 +298,94 @@
   </si>
   <si>
     <t>Inputparameter Merit-Order-Modell</t>
+  </si>
+  <si>
+    <t>Uran</t>
+  </si>
+  <si>
+    <t>Brennstoffe</t>
+  </si>
+  <si>
+    <r>
+      <t>Brennstoffkosten  [€/MWh</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Emissionsfaktor [t CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/MWh</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Wirkungsgrad</t>
+  </si>
+  <si>
+    <t>Kraftwerke</t>
+  </si>
+  <si>
+    <t>Kapazität</t>
   </si>
 </sst>
 </file>
@@ -328,7 +396,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +431,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -488,10 +564,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -516,6 +591,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -808,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9F5ADF-242F-44CD-878A-25895C987D0F}">
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -822,254 +899,254 @@
   <sheetData>
     <row r="2" spans="2:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="23"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="24"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>54.06</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="21"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B5" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="3" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="4"/>
+      <c r="C17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="6">
-        <v>14.56</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="8">
-        <v>54.06</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="3" t="s">
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B14" s="7" t="s">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0.54</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.51</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B17" s="5"/>
-      <c r="C17" s="10" t="s">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="17">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="13">
-        <v>0.39500000000000002</v>
-      </c>
-      <c r="D18" s="13">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="E18" s="14">
-        <v>0.308</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="13">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="E19" s="14">
-        <v>0.29499999999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="15">
-        <v>0.54</v>
-      </c>
-      <c r="D20" s="15">
-        <v>0.51</v>
-      </c>
-      <c r="E20" s="16">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="17">
-        <v>0.40699999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="17">
-        <v>0.33500000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0.20200000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="6">
+      <c r="B28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5">
         <v>5.5</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="19">
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="18">
         <f>$C$9/$C$18+$C$23/$C$18*$C$14</f>
         <v>61.427848101265816</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="19">
+      <c r="B30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="18">
         <f>$C$9/$D$18+$C$23/$D$18*$C$14</f>
         <v>70.127167630057798</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="19">
+      <c r="B31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="18">
         <f>$C$9/$E$18+$C$23/$E$18*$C$14</f>
         <v>78.779220779220779</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B32" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="19">
+      <c r="B32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="18">
         <f>$C$10/$C$19+$C$24/$C$19*$C$14</f>
         <v>82.210796915167094</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="19">
+      <c r="B33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="18">
         <f>$C$10/$D$19+$C$24/$D$19*$C$14</f>
         <v>95.462686567164184</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B34" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="19">
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="18">
         <f>$C$10/$E$19+$C$24/$E$19*$C$14</f>
         <v>108.40677966101696</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="19">
+      <c r="B35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="18">
         <f>$C$11/$C$20+$C$25/$C$20*$C$14</f>
         <v>119.56296296296297</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="19">
+      <c r="B36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="18">
         <f>$C$11/$D$20+$C$25/$D$20*$C$14</f>
         <v>126.59607843137255</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B37" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="20">
+      <c r="B37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="19">
         <f>$C$11/$E$20+$C$25/$E$20*$C$14</f>
         <v>140.35652173913044</v>
       </c>
@@ -1087,70 +1164,269 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462A2DE2-E034-4F83-9F51-3596A9040BF8}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="G2">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="G3">
+        <v>14100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="G4">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0.308</v>
+      </c>
+      <c r="G5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="G6">
+        <v>13300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G8">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0.54</v>
+      </c>
+      <c r="G9">
+        <v>17700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0.51</v>
+      </c>
+      <c r="G10">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="20">
+        <v>0.46</v>
+      </c>
+      <c r="G11">
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
@@ -1159,161 +1435,86 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA14E8B2-0A04-4EA8-A66C-564981641E2D}">
-  <dimension ref="A1:A11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DCFAA9-C271-4DEB-9262-0F38203DC12E}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.46484375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <f>Cockpit!C28</f>
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
-        <f>Cockpit!C29</f>
-        <v>61.427848101265816</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <f>Cockpit!C30</f>
-        <v>70.127167630057798</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
-        <f>Cockpit!C31</f>
-        <v>78.779220779220779</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
-        <f>Cockpit!C32</f>
-        <v>82.210796915167094</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" s="2">
-        <f>Cockpit!C33</f>
-        <v>95.462686567164184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" s="2">
-        <f>Cockpit!C34</f>
-        <v>108.40677966101696</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" s="2">
-        <f>Cockpit!C35</f>
-        <v>119.56296296296297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" s="2">
-        <f>Cockpit!C36</f>
-        <v>126.59607843137255</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" s="2">
-        <f>Cockpit!C37</f>
-        <v>140.35652173913044</v>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>3.1</v>
+      </c>
+      <c r="C3">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>14.56</v>
+      </c>
+      <c r="C4">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>54.06</v>
+      </c>
+      <c r="C5">
+        <v>0.20200000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>8100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>14100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>13300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>17700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>8000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503AA485-0496-4332-9891-D6E32C8F4635}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1324,10 +1525,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>